<commit_message>
Actualización de archivos locales recuperados
Actualización de archivos locales recuperados
</commit_message>
<xml_diff>
--- a/data/Autores.xlsx
+++ b/data/Autores.xlsx
@@ -1,24 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos Sarmiento\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C95D1D7-2E99-43C3-AB86-EFE0F6277081}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C95D1D7-2E99-43C3-AB86-EFE0F6277081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{B664BAEF-DAC7-4489-BFDC-E2F89FC333A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -114,13 +125,13 @@
     <t>jcrodriguez@umich.mx</t>
   </si>
   <si>
+    <t>+52 (443) 179-6976</t>
+  </si>
+  <si>
+    <t>Mario Gómez</t>
+  </si>
+  <si>
     <t>mgomez@umich.mx</t>
-  </si>
-  <si>
-    <t>+52 (443) 179-6976</t>
-  </si>
-  <si>
-    <t>Mario Gómez</t>
   </si>
   <si>
     <t>+52 (443) 185-2214</t>
@@ -157,7 +168,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,7 +272,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -563,14 +574,14 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="36.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.109375" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -581,7 +592,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -590,7 +601,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" s="5" customFormat="1">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -601,7 +612,7 @@
         <v>9831540968</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" s="5" customFormat="1">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
@@ -612,7 +623,7 @@
         <v>4145977410</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" s="5" customFormat="1">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -623,7 +634,7 @@
         <v>573014989039</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" s="5" customFormat="1">
       <c r="A6" s="6" t="s">
         <v>11</v>
       </c>
@@ -634,7 +645,7 @@
         <v>51956159061</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" s="5" customFormat="1">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -645,7 +656,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" s="5" customFormat="1">
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
@@ -656,7 +667,7 @@
         <v>573142438565</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" s="5" customFormat="1">
       <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
@@ -667,7 +678,7 @@
         <v>996023727</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" s="5" customFormat="1">
       <c r="A10" s="6" t="s">
         <v>20</v>
       </c>
@@ -678,7 +689,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" s="5" customFormat="1">
       <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
@@ -689,7 +700,7 @@
         <v>999950618</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" s="5" customFormat="1">
       <c r="A12" s="6" t="s">
         <v>25</v>
       </c>
@@ -700,7 +711,7 @@
         <v>984594080</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" s="5" customFormat="1">
       <c r="A13" s="4" t="s">
         <v>27</v>
       </c>
@@ -708,21 +719,21 @@
         <v>28</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+      <c r="B14" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>29</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3">
       <c r="A15" s="4" t="s">
         <v>33</v>
       </c>
@@ -733,7 +744,7 @@
         <v>3152421451</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" s="5" customFormat="1">
       <c r="A16" s="6" t="s">
         <v>35</v>
       </c>
@@ -744,7 +755,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" s="5" customFormat="1">
       <c r="A17" s="4" t="s">
         <v>38</v>
       </c>
@@ -755,7 +766,7 @@
         <v>51936833185</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" s="5" customFormat="1">
       <c r="A18" s="6" t="s">
         <v>40</v>
       </c>

</xml_diff>